<commit_message>
forgot to upload the conductivity data!
</commit_message>
<xml_diff>
--- a/Data/well_sampling.xlsx
+++ b/Data/well_sampling.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f24a4ec7a36d250/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f24a4ec7a36d250/Documents/SL_chloride/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99CC51DC-500A-492A-AEE9-1F8EB78312A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{99CC51DC-500A-492A-AEE9-1F8EB78312A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89C548BE-93EA-4369-AC3D-FEC3567AADD2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5037A25F-07C1-4D38-AD00-C4B58C6F2106}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>sampledate</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>well 5 dup</t>
+  </si>
+  <si>
+    <t>actual_conductivity</t>
+  </si>
+  <si>
+    <t>temp</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6819BE3-BC79-451F-9696-DF41EE0F6E3E}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,9 +436,10 @@
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,45 +455,81 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44029.513888888891</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="F2">
+        <v>26.57</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44029.524305555555</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="F3">
+        <v>37.090000000000003</v>
+      </c>
+      <c r="G3">
+        <v>12.9</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44029.533333333333</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="F4">
+        <v>484.9</v>
+      </c>
+      <c r="G4">
+        <v>13.2</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44029.543055555558</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="F5">
+        <v>58.86</v>
+      </c>
+      <c r="G5">
+        <v>13.4</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44029.547222222223</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
+      </c>
+      <c r="F6">
+        <v>57.59</v>
+      </c>
+      <c r="G6">
+        <v>12.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added well depths and water depths to .xslx
</commit_message>
<xml_diff>
--- a/Data/well_sampling.xlsx
+++ b/Data/well_sampling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f24a4ec7a36d250/Documents/SL_chloride/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{99CC51DC-500A-492A-AEE9-1F8EB78312A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89C548BE-93EA-4369-AC3D-FEC3567AADD2}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="5_{30B9BAD9-3068-48BC-94F4-795BBB7EF451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0DDE1C73-13E5-4E8B-9FC6-D52B3172E98D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5037A25F-07C1-4D38-AD00-C4B58C6F2106}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5037A25F-07C1-4D38-AD00-C4B58C6F2106}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>sampledate</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>temp</t>
+  </si>
+  <si>
+    <t>water_depth</t>
+  </si>
+  <si>
+    <t>well_depth</t>
   </si>
 </sst>
 </file>
@@ -424,22 +430,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6819BE3-BC79-451F-9696-DF41EE0F6E3E}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,8 +469,14 @@
       <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44029.513888888891</v>
       </c>
@@ -475,8 +489,14 @@
       <c r="G2">
         <v>14</v>
       </c>
+      <c r="H2">
+        <v>132</v>
+      </c>
+      <c r="I2">
+        <v>236</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44029.524305555555</v>
       </c>
@@ -489,8 +509,14 @@
       <c r="G3">
         <v>12.9</v>
       </c>
+      <c r="H3">
+        <v>261</v>
+      </c>
+      <c r="I3">
+        <v>388</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44029.533333333333</v>
       </c>
@@ -503,8 +529,14 @@
       <c r="G4">
         <v>13.2</v>
       </c>
+      <c r="H4">
+        <v>287</v>
+      </c>
+      <c r="I4">
+        <v>639</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44029.543055555558</v>
       </c>
@@ -517,8 +549,14 @@
       <c r="G5">
         <v>13.4</v>
       </c>
+      <c r="H5">
+        <v>45</v>
+      </c>
+      <c r="I5">
+        <v>130</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44029.547222222223</v>
       </c>
@@ -530,6 +568,12 @@
       </c>
       <c r="G6">
         <v>12.7</v>
+      </c>
+      <c r="H6">
+        <v>45</v>
+      </c>
+      <c r="I6">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>